<commit_message>
actualizadas las cabeceras de los reportes
segun las ultimas correciones
todos los reportes a dia segun las ultimas correcciones
</commit_message>
<xml_diff>
--- a/plantilla_promotor.xlsx
+++ b/plantilla_promotor.xlsx
@@ -113,7 +113,7 @@
     <t xml:space="preserve">Fecha Preliquidación:</t>
   </si>
   <si>
-    <t xml:space="preserve">Número exterior:</t>
+    <t xml:space="preserve">Cuneta bancaria dada de alta:</t>
   </si>
 </sst>
 </file>
@@ -403,9 +403,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>534600</xdr:colOff>
+      <xdr:colOff>534240</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>119520</xdr:rowOff>
+      <xdr:rowOff>119160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -419,7 +419,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1161720" cy="294480"/>
+          <a:ext cx="1161360" cy="294120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -442,10 +442,10 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.17"/>

</xml_diff>